<commit_message>
1.5.0 forCBegin forCEnd循环多个单元格;ifCBegin ifCEnd条件单元格
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>序号</t>
   </si>
@@ -336,26 +336,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>%var isTr = true;%&gt;</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;%ifRBegin isTr%&gt;</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">&lt;%ifRBegin </t>
     </r>
     <r>
@@ -459,6 +439,33 @@
       </rPr>
       <t>%&gt;</t>
     </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%var isTr = true;%&gt;</t>
+  </si>
+  <si>
+    <t>&lt;%forRBegin key in ["key1","key2"]%&gt;&lt;%ifRBegin isTr%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%ifREnd%&gt;&lt;%forREnd%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%forCEnd%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%ifCEnd%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%ifCBegin false%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%forCBegin str in ["a","b"]%&gt;&lt;%=str%&gt;</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -469,7 +476,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -533,8 +540,14 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +578,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -598,7 +623,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -677,6 +702,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1023,10 +1060,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1383,44 +1420,65 @@
         <v>31</v>
       </c>
     </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="A24" s="14"/>
       <c r="C24" s="14"/>
       <c r="E24" s="14"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:12" s="22" customFormat="1">
       <c r="A25" s="23" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H25" s="23"/>
       <c r="J25" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="28" customFormat="1">
+      <c r="C26" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="14"/>
+    </row>
+    <row r="30" spans="1:12" s="27" customFormat="1">
+      <c r="A30" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="27" customFormat="1">
-      <c r="A28" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="24" customFormat="1"/>
-    <row r="30" spans="1:12" s="25" customFormat="1"/>
-    <row r="31" spans="1:12">
-      <c r="A31" s="14" t="s">
-        <v>52</v>
+    <row r="31" spans="1:12" s="24" customFormat="1"/>
+    <row r="32" spans="1:12" s="25" customFormat="1"/>
+    <row r="33" spans="1:1">
+      <c r="A33" s="14" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3.6.2 输出日期格式(设置单元格为日期格式):<%~new Date("2019-09-08 22:12:31")%>
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hugjs\ejsExcel\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hugjs\ejsExcel\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BE96CF-1639-4E99-B5D1-25B22A0AC1BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40375219-DC96-4C29-8669-3CE2CD11BA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2772" windowWidth="14688" windowHeight="4200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="申请单" sheetId="4" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="被删除的工作表" sheetId="8" r:id="rId4"/>
     <sheet name="被显示的工作表" sheetId="9" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>序号</t>
   </si>
@@ -39,10 +39,6 @@
   </si>
   <si>
     <t>批准:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>审核:</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -635,6 +631,14 @@
   </si>
   <si>
     <t>&lt;%ifCEnd%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%~new Date("2019-09-08 22:12:31")%&gt;</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>输出日期格式(设置单元格为日期格式):</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -712,6 +716,7 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -719,6 +724,7 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -784,7 +790,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -857,6 +863,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1251,34 +1260,34 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.8984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="3.69921875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.59765625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.59765625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.8984375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.19921875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.6875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="5.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.1875" style="3" customWidth="1"/>
     <col min="9" max="9" width="5.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.1875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="3" customWidth="1"/>
     <col min="13" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3">
         <v>1</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1290,19 +1299,19 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1312,61 +1321,61 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="15" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:16" s="15" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <f>SUM(A1,A2)</f>
         <v>3</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="17" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>17</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="17"/>
       <c r="K3" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:16" ht="24" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="4.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:16" ht="25.5" x14ac:dyDescent="0.4">
       <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>1</v>
@@ -1378,33 +1387,33 @@
         <v>3</v>
       </c>
       <c r="J5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="L5" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>23</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -1413,12 +1422,12 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -1431,11 +1440,11 @@
       <c r="K7" s="9"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="10"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -1446,10 +1455,10 @@
       <c r="K8" s="9"/>
       <c r="L8" s="12"/>
       <c r="M8" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="10"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1462,12 +1471,12 @@
       <c r="K9" s="9"/>
       <c r="L9" s="12"/>
       <c r="M9" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="9"/>
@@ -1476,14 +1485,14 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="11"/>
       <c r="K10" s="9"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1496,13 +1505,13 @@
       <c r="K11" s="9"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -1514,7 +1523,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="10"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1527,7 +1536,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="10"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1540,7 +1549,7 @@
       <c r="K14" s="9"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="10"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1553,7 +1562,7 @@
       <c r="K15" s="9"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="10"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1566,7 +1575,7 @@
       <c r="K16" s="9"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="2:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="10"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1579,124 +1588,126 @@
       <c r="K17" s="9"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="2:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="5"/>
       <c r="C18" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>25</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>26</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>70</v>
+      </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L18" s="7"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.4">
       <c r="C20" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.4">
       <c r="L21" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M21" s="14"/>
       <c r="P21" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.4">
       <c r="L22" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.4">
       <c r="C24" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.4">
       <c r="C25" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.4">
       <c r="C28" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C32" s="14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C32" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="I32" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C33" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C34" s="14" t="str">
         <f>"&lt;%="&amp;C33&amp;"%&gt;"</f>
         <v>&lt;%=fld1%&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="C37" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="C38" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="C39" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="C40" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="C41" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C39" s="3" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A44" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C41" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="K44" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A45" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1720,7 +1731,7 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1735,16 +1746,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1759,16 +1770,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1783,16 +1794,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>